<commit_message>
Update on scrum docs
</commit_message>
<xml_diff>
--- a/Scrum/Proyect/Sprint-Backlog v2.xlsx
+++ b/Scrum/Proyect/Sprint-Backlog v2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\documents\Proyectos\dotNet\Report_Game_Statistic\_Report_Game_Statistic_\Scrum\Proyect\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\documents\Proyectos\dotNet\Report_Game_Statistic\_Report_Game_Statistic_\ReportGameStats\Scrum\Proyect\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint1" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="38">
   <si>
     <t>Product Backlog Item</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>As a user of DGS I need to use the system to insert start date, end date and on the system, also LogIdUser, so I can save a registry of these activities</t>
+  </si>
+  <si>
+    <t>https://github.com/Luigig8per/CACtiveMQSubscribe</t>
   </si>
 </sst>
 </file>
@@ -232,7 +235,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="26">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -259,8 +262,9 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -279,12 +283,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="23" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -294,8 +292,15 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="25" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="26"/>
   </cellXfs>
-  <cellStyles count="26">
+  <cellStyles count="27">
     <cellStyle name="Accent2" xfId="25" builtinId="33"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -320,6 +325,7 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8"/>
     <cellStyle name="Neutral" xfId="24" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -461,11 +467,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1105285024"/>
-        <c:axId val="-1105284480"/>
+        <c:axId val="717967408"/>
+        <c:axId val="717970128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1105285024"/>
+        <c:axId val="717967408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -475,7 +481,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1105284480"/>
+        <c:crossAx val="717970128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -483,7 +489,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1105284480"/>
+        <c:axId val="717970128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -494,7 +500,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1105285024"/>
+        <c:crossAx val="717967408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -843,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -863,7 +869,7 @@
     <col min="14" max="16384" width="12" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -907,11 +913,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -951,9 +957,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="8"/>
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="B3" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -993,9 +999,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="12" t="s">
+    <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
+      <c r="B4" s="10" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1035,9 +1041,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10" t="s">
+    <row r="5" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -1076,10 +1082,13 @@
       <c r="O5" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10" t="s">
+      <c r="Q5" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1119,8 +1128,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="9"/>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="12"/>
       <c r="B7" s="4" t="s">
         <v>20</v>
       </c>
@@ -1161,8 +1170,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="12"/>
       <c r="B8" s="4" t="s">
         <v>25</v>
       </c>
@@ -1203,7 +1212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="7" t="s">
         <v>26</v>
@@ -1245,7 +1254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="7" t="s">
         <v>27</v>
@@ -1288,7 +1297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B11" s="7" t="s">
         <v>28</v>
       </c>
@@ -1329,7 +1338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="7" t="s">
         <v>29</v>
@@ -1371,8 +1380,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B13" s="10" t="s">
+    <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1412,8 +1421,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B14" s="11" t="s">
+    <row r="14" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1453,7 +1462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
         <v>32</v>
       </c>
@@ -1494,7 +1503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B16" s="7" t="s">
         <v>33</v>
       </c>
@@ -1536,7 +1545,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -1577,7 +1586,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -1680,9 +1689,12 @@
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A8"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="Q5" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1692,6 +1704,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -1737,19 +1758,7 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?><p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"><documentManagement><_dlc_DocId xmlns="0d93dc7d-5998-434b-bf34-aa89b432ec07">WORK-769-153</_dlc_DocId><_dlc_DocIdUrl xmlns="0d93dc7d-5998-434b-bf34-aa89b432ec07"><Url>http://intranet/workingtogether/projects/110405/_layouts/DocIdRedir.aspx?ID=WORK-769-153</Url><Description>WORK-769-153</Description></_dlc_DocIdUrl><IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/><Last_x0020_Archive xmlns="$ListId:Shared Documents;" xsi:nil="true"/><Reason xmlns="$ListId:Shared Documents;" xsi:nil="true"></Reason></documentManagement></p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?><ct:contentTypeSchema ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F770ABC8F9B27C4C8461F4575C23FAEA" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6f0f4afd6cc55b40f57cb0d59e49aa45" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes">
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?><ct:contentTypeSchema ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F770ABC8F9B27C4C8461F4575C23FAEA" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6f0f4afd6cc55b40f57cb0d59e49aa45" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes">
 <xsd:schema targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f7c28edf12e174e47f2c7bd2736e8bd" ns2:_="" ns3:_="" ns4:_="" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0d93dc7d-5998-434b-bf34-aa89b432ec07" xmlns:ns3="$ListId:Shared Documents;" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v4">
 <xsd:import namespace="0d93dc7d-5998-434b-bf34-aa89b432ec07"/>
 <xsd:import namespace="$ListId:Shared Documents;"/>
@@ -1923,7 +1932,18 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?><p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"><documentManagement><_dlc_DocId xmlns="0d93dc7d-5998-434b-bf34-aa89b432ec07">WORK-769-153</_dlc_DocId><_dlc_DocIdUrl xmlns="0d93dc7d-5998-434b-bf34-aa89b432ec07"><Url>http://intranet/workingtogether/projects/110405/_layouts/DocIdRedir.aspx?ID=WORK-769-153</Url><Description>WORK-769-153</Description></_dlc_DocIdUrl><IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/><Last_x0020_Archive xmlns="$ListId:Shared Documents;" xsi:nil="true"/><Reason xmlns="$ListId:Shared Documents;" xsi:nil="true"></Reason></documentManagement></p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2B9EEEF-7393-4E57-9716-D967A23AC816}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F807D2B-FCE5-4B63-BC9A-551BEF173D66}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
@@ -1931,33 +1951,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2B9EEEF-7393-4E57-9716-D967A23AC816}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47BCCC64-3980-40D2-8C4F-F5BACE67ECB4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="$ListId:Shared Documents;"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="0d93dc7d-5998-434b-bf34-aa89b432ec07"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0008E140-BD0E-4C41-947D-F18B1A1E4B6B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1975,4 +1969,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47BCCC64-3980-40D2-8C4F-F5BACE67ECB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="$ListId:Shared Documents;"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="0d93dc7d-5998-434b-bf34-aa89b432ec07"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Now can select leagues on combobox
</commit_message>
<xml_diff>
--- a/Scrum/Proyect/Sprint-Backlog v2.xlsx
+++ b/Scrum/Proyect/Sprint-Backlog v2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="41">
   <si>
     <t>Product Backlog Item</t>
   </si>
@@ -138,6 +138,15 @@
   </si>
   <si>
     <t>https://github.com/Luigig8per/CACtiveMQSubscribe</t>
+  </si>
+  <si>
+    <t>Need to show the data on ASP.net</t>
+  </si>
+  <si>
+    <t>Its already working on desktop</t>
+  </si>
+  <si>
+    <t>Task 8 - Load leagues on cboBox</t>
   </si>
 </sst>
 </file>
@@ -292,13 +301,13 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="25" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="26"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="26"/>
   </cellXfs>
   <cellStyles count="27">
     <cellStyle name="Accent2" xfId="25" builtinId="33"/>
@@ -467,11 +476,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="717967408"/>
-        <c:axId val="717970128"/>
+        <c:axId val="-1680340368"/>
+        <c:axId val="-1680340912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="717967408"/>
+        <c:axId val="-1680340368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -481,7 +490,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="717970128"/>
+        <c:crossAx val="-1680340912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -489,7 +498,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="717970128"/>
+        <c:axId val="-1680340912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -500,7 +509,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="717967408"/>
+        <c:crossAx val="-1680340368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -852,7 +861,7 @@
   <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -914,7 +923,7 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -958,7 +967,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="8" t="s">
         <v>14</v>
       </c>
@@ -1000,7 +1009,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="10" t="s">
         <v>17</v>
       </c>
@@ -1042,7 +1051,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="8" t="s">
         <v>18</v>
       </c>
@@ -1082,12 +1091,12 @@
       <c r="O5" s="1">
         <v>0</v>
       </c>
-      <c r="Q5" s="13" t="s">
+      <c r="Q5" s="11" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="8" t="s">
         <v>19</v>
       </c>
@@ -1129,7 +1138,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="4" t="s">
         <v>20</v>
       </c>
@@ -1170,9 +1179,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="12"/>
-      <c r="B8" s="4" t="s">
+    <row r="8" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1210,6 +1219,9 @@
       </c>
       <c r="O8" s="1">
         <v>0</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -1252,6 +1264,9 @@
       </c>
       <c r="O9" s="1">
         <v>0</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1672,6 +1687,14 @@
       <c r="O22" s="2">
         <f>SUM(O2:O8)</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B27" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Extracting results from MAJOR LEAGUE BASEBALL
Added param to select league. Param is passed as a string.

-= Actually working =-
</commit_message>
<xml_diff>
--- a/Scrum/Proyect/Sprint-Backlog v2.xlsx
+++ b/Scrum/Proyect/Sprint-Backlog v2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="43">
   <si>
     <t>Product Backlog Item</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>Task 8 - Load leagues on cboBox</t>
+  </si>
+  <si>
+    <t>Task 9 - Load SP with leagues parameter</t>
+  </si>
+  <si>
+    <t>Task 10 - Extract to excel</t>
   </si>
 </sst>
 </file>
@@ -476,11 +482,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1680340368"/>
-        <c:axId val="-1680340912"/>
+        <c:axId val="-201367472"/>
+        <c:axId val="-201360400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1680340368"/>
+        <c:axId val="-201367472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -490,7 +496,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1680340912"/>
+        <c:crossAx val="-201360400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -498,7 +504,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1680340912"/>
+        <c:axId val="-201360400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -509,7 +515,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1680340368"/>
+        <c:crossAx val="-201367472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -861,7 +867,7 @@
   <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1689,12 +1695,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B27" s="4" t="s">
+    <row r="27" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="B27" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E27" s="1">
         <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B28" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B29" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" s="1">
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
@@ -1727,15 +1749,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -1781,7 +1794,19 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?><ct:contentTypeSchema ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F770ABC8F9B27C4C8461F4575C23FAEA" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6f0f4afd6cc55b40f57cb0d59e49aa45" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes">
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?><p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"><documentManagement><_dlc_DocId xmlns="0d93dc7d-5998-434b-bf34-aa89b432ec07">WORK-769-153</_dlc_DocId><_dlc_DocIdUrl xmlns="0d93dc7d-5998-434b-bf34-aa89b432ec07"><Url>http://intranet/workingtogether/projects/110405/_layouts/DocIdRedir.aspx?ID=WORK-769-153</Url><Description>WORK-769-153</Description></_dlc_DocIdUrl><IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/><Last_x0020_Archive xmlns="$ListId:Shared Documents;" xsi:nil="true"/><Reason xmlns="$ListId:Shared Documents;" xsi:nil="true"></Reason></documentManagement></p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?><ct:contentTypeSchema ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F770ABC8F9B27C4C8461F4575C23FAEA" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6f0f4afd6cc55b40f57cb0d59e49aa45" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes">
 <xsd:schema targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f7c28edf12e174e47f2c7bd2736e8bd" ns2:_="" ns3:_="" ns4:_="" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0d93dc7d-5998-434b-bf34-aa89b432ec07" xmlns:ns3="$ListId:Shared Documents;" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v4">
 <xsd:import namespace="0d93dc7d-5998-434b-bf34-aa89b432ec07"/>
 <xsd:import namespace="$ListId:Shared Documents;"/>
@@ -1955,10 +1980,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?><p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"><documentManagement><_dlc_DocId xmlns="0d93dc7d-5998-434b-bf34-aa89b432ec07">WORK-769-153</_dlc_DocId><_dlc_DocIdUrl xmlns="0d93dc7d-5998-434b-bf34-aa89b432ec07"><Url>http://intranet/workingtogether/projects/110405/_layouts/DocIdRedir.aspx?ID=WORK-769-153</Url><Description>WORK-769-153</Description></_dlc_DocIdUrl><IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/><Last_x0020_Archive xmlns="$ListId:Shared Documents;" xsi:nil="true"/><Reason xmlns="$ListId:Shared Documents;" xsi:nil="true"></Reason></documentManagement></p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F807D2B-FCE5-4B63-BC9A-551BEF173D66}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2B9EEEF-7393-4E57-9716-D967A23AC816}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -1966,15 +1996,25 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F807D2B-FCE5-4B63-BC9A-551BEF173D66}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47BCCC64-3980-40D2-8C4F-F5BACE67ECB4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="$ListId:Shared Documents;"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="0d93dc7d-5998-434b-bf34-aa89b432ec07"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0008E140-BD0E-4C41-947D-F18B1A1E4B6B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1992,22 +2032,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47BCCC64-3980-40D2-8C4F-F5BACE67ECB4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="$ListId:Shared Documents;"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="0d93dc7d-5998-434b-bf34-aa89b432ec07"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>